<commit_message>
Closing prices instead of current
</commit_message>
<xml_diff>
--- a/stock_grabber/fake_finances.xlsx
+++ b/stock_grabber/fake_finances.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dan.donohue\Desktop\Projects\python\stock_grabber\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
   </bookViews>
   <sheets>
-    <sheet name="AwesomeSheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="AwesomeSheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Dan's Fake Money Supply</t>
   </si>
@@ -34,9 +39,6 @@
     <t>Shares</t>
   </si>
   <si>
-    <t>Current Price</t>
-  </si>
-  <si>
     <t>Day's Gain</t>
   </si>
   <si>
@@ -73,68 +75,71 @@
     <t>SQ</t>
   </si>
   <si>
-    <t>+1.65%</t>
+    <t>-0.47%</t>
   </si>
   <si>
     <t>Total Money Supply</t>
   </si>
   <si>
     <t>ETH</t>
+  </si>
+  <si>
+    <t>Prev Close</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@" numFmtId="164"/>
+    <numFmt numFmtId="164" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <color rgb="FF000000"/>
-      <sz val="12"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <b val="1"/>
-      <color rgb="FF000000"/>
-      <sz val="18"/>
     </font>
     <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <b val="1"/>
-      <color rgb="FF000000"/>
-      <sz val="12"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <color rgb="FF000000"/>
-      <sz val="12"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <b val="1"/>
-      <color rgb="FF000000"/>
-      <sz val="18"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color rgb="FF000000"/>
-      <sz val="12"/>
     </font>
     <font>
+      <sz val="13"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color rgb="FF000000"/>
-      <sz val="13"/>
     </font>
   </fonts>
   <fills count="4">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -162,47 +167,47 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="17">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="2" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="9" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
-    <cellStyle builtinId="5" name="Percent" xfId="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -216,7 +221,15 @@
       </font>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -482,45 +495,48 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15.6" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="15" width="27.69921875"/>
-    <col customWidth="1" max="2" min="2" style="15" width="18.09765625"/>
-    <col customWidth="1" max="3" min="3" style="15" width="22.09765625"/>
-    <col customWidth="1" max="4" min="4" style="15" width="19"/>
-    <col customWidth="1" max="5" min="5" style="15" width="11.09765625"/>
-    <col bestFit="1" customWidth="1" max="6" min="6" style="15" width="12.59765625"/>
-    <col customWidth="1" max="7" min="7" style="15" width="15.59765625"/>
-    <col customWidth="1" max="8" min="8" style="15" width="17.3984375"/>
-    <col bestFit="1" customWidth="1" max="9" min="9" style="15" width="14.8984375"/>
-    <col customWidth="1" max="10" min="10" style="15" width="13"/>
-    <col customWidth="1" max="11" min="11" style="15" width="12.19921875"/>
+    <col min="1" max="1" width="27.69921875" style="12" customWidth="1"/>
+    <col min="2" max="2" width="18.09765625" style="12" customWidth="1"/>
+    <col min="3" max="3" width="22.09765625" style="12" customWidth="1"/>
+    <col min="4" max="4" width="19" style="12" customWidth="1"/>
+    <col min="5" max="5" width="11.09765625" style="12" customWidth="1"/>
+    <col min="6" max="6" width="12.59765625" style="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.59765625" style="12" customWidth="1"/>
+    <col min="8" max="8" width="17.3984375" style="12" customWidth="1"/>
+    <col min="9" max="9" width="14.8984375" style="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13" style="12" customWidth="1"/>
+    <col min="11" max="11" width="12.19921875" style="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="23.4" r="1" s="15" spans="1:12">
+    <row r="1" spans="1:12" ht="23.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
       <c r="D1" s="16" t="s">
         <v>1</v>
       </c>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
     </row>
-    <row customHeight="1" ht="17.4" r="2" s="15" spans="1:12">
+    <row r="2" spans="1:12" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="n">
+      <c r="B2" s="2">
         <v>2000</v>
       </c>
       <c r="D2" s="8" t="s">
@@ -533,156 +549,156 @@
         <v>5</v>
       </c>
       <c r="G2" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="I2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="K2" s="9" t="n"/>
-      <c r="L2" s="9" t="n"/>
-    </row>
-    <row r="3" spans="1:12">
-      <c r="A3" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="B3" s="2">
         <f>SUM(E3:E6)</f>
-        <v/>
+        <v>5478.5</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E3" s="4">
         <f>SUM(F3*G3)</f>
-        <v/>
-      </c>
-      <c r="F3" t="n">
+        <v>1489.8</v>
+      </c>
+      <c r="F3">
         <v>10</v>
       </c>
-      <c r="G3" t="n">
-        <v>145.42</v>
+      <c r="G3">
+        <v>148.97999999999999</v>
       </c>
       <c r="H3" s="11">
         <f>SUM(E3*(I3))</f>
-        <v/>
+        <v>-35.60622</v>
       </c>
       <c r="I3" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:12">
-      <c r="A4" s="5" t="s">
+      <c r="B4" s="2">
+        <v>9703.9599999999991</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>12</v>
-      </c>
-      <c r="B4" s="2" t="n">
-        <v>9703.959999999999</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>13</v>
       </c>
       <c r="E4" s="4">
         <f>SUM(F4*G4)</f>
-        <v/>
-      </c>
-      <c r="F4" t="n">
+        <v>2788.8</v>
+      </c>
+      <c r="F4">
         <v>20</v>
       </c>
-      <c r="G4" t="n">
-        <v>139.08</v>
+      <c r="G4">
+        <v>139.44</v>
       </c>
       <c r="H4" s="11">
         <f>SUM(E4*(I4))</f>
-        <v/>
+        <v>-7.2508800000000004</v>
       </c>
       <c r="I4" s="10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
-      <c r="A5" s="5" t="s">
-        <v>15</v>
       </c>
       <c r="B5" s="2">
         <f>SUM(E7)</f>
-        <v/>
+        <v>797.29</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E5" s="4">
         <f>SUM(F5*G5)</f>
-        <v/>
-      </c>
-      <c r="F5" t="n">
+        <v>255.89999999999998</v>
+      </c>
+      <c r="F5">
         <v>30</v>
       </c>
-      <c r="G5" t="n">
-        <v>8.529999999999999</v>
+      <c r="G5">
+        <v>8.5299999999999994</v>
       </c>
       <c r="H5" s="11">
         <f>SUM(E5*(I5))</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="I5" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D6" s="3" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12">
-      <c r="D6" s="3" t="s">
-        <v>18</v>
       </c>
       <c r="E6" s="4">
         <f>SUM(F6*G6)</f>
-        <v/>
-      </c>
-      <c r="F6" t="n">
+        <v>944</v>
+      </c>
+      <c r="F6">
         <v>40</v>
       </c>
-      <c r="G6" t="n">
-        <v>23.41</v>
+      <c r="G6">
+        <v>23.6</v>
       </c>
       <c r="H6" s="11">
         <f>SUM(E6*(I6))</f>
-        <v/>
+        <v>-4.4367999999999999</v>
       </c>
       <c r="I6" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12">
-      <c r="A7" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="B7" s="6">
         <f>SUM(B5+B4+B3+B2)</f>
-        <v/>
+        <v>17979.75</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E7" s="4">
         <f>SUM(F7*G7)</f>
-        <v/>
-      </c>
-      <c r="F7" t="n">
+        <v>797.29</v>
+      </c>
+      <c r="F7">
         <v>2</v>
       </c>
-      <c r="G7" t="n">
-        <v>391.221</v>
+      <c r="G7">
+        <v>398.64499999999998</v>
       </c>
       <c r="H7" s="11">
         <f>SUM(E7*(I7))</f>
-        <v/>
-      </c>
-      <c r="I7" s="10" t="n">
-        <v>0.0597</v>
+        <v>80.127645000000001</v>
+      </c>
+      <c r="I7" s="10">
+        <v>0.10050000000000001</v>
       </c>
     </row>
-    <row customHeight="1" ht="23.4" r="16" s="15" spans="1:12">
-      <c r="G16" s="16" t="n"/>
+    <row r="16" spans="1:12" ht="23.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="G16" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -690,14 +706,14 @@
     <mergeCell ref="D1:I1"/>
   </mergeCells>
   <conditionalFormatting sqref="H3:H7">
-    <cfRule dxfId="1" operator="lessThan" priority="2" type="cellIs">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule dxfId="0" operator="greaterThan" priority="1" type="cellIs">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Finished bookstore part 1
</commit_message>
<xml_diff>
--- a/stock_grabber/fake_finances.xlsx
+++ b/stock_grabber/fake_finances.xlsx
@@ -49,7 +49,7 @@
     <t>AAPL</t>
   </si>
   <si>
-    <t>-2.39%</t>
+    <t>-0.60%</t>
   </si>
   <si>
     <t>Vanguard 500 Index Fund</t>
@@ -58,7 +58,7 @@
     <t xml:space="preserve">BABA </t>
   </si>
   <si>
-    <t>-0.26%</t>
+    <t>-1.16%</t>
   </si>
   <si>
     <t>Etherium</t>
@@ -67,13 +67,13 @@
     <t>GPRO</t>
   </si>
   <si>
-    <t>+1.91%</t>
+    <t>-3.24%</t>
   </si>
   <si>
     <t>SQ</t>
   </si>
   <si>
-    <t>-0.30%</t>
+    <t>-1.92%</t>
   </si>
   <si>
     <t>Total Money Supply</t>
@@ -563,7 +563,7 @@
         <v>10</v>
       </c>
       <c r="G3" t="n">
-        <v>148.98</v>
+        <v>145.16</v>
       </c>
       <c r="H3" s="11">
         <f>SUM(E3*(I3))</f>
@@ -591,7 +591,7 @@
         <v>20</v>
       </c>
       <c r="G4" t="n">
-        <v>139.44</v>
+        <v>136.67</v>
       </c>
       <c r="H4" s="11">
         <f>SUM(E4*(I4))</f>
@@ -620,7 +620,7 @@
         <v>30</v>
       </c>
       <c r="G5" t="n">
-        <v>8.369999999999999</v>
+        <v>8.34</v>
       </c>
       <c r="H5" s="11">
         <f>SUM(E5*(I5))</f>
@@ -642,7 +642,7 @@
         <v>40</v>
       </c>
       <c r="G6" t="n">
-        <v>23.6</v>
+        <v>23.99</v>
       </c>
       <c r="H6" s="11">
         <f>SUM(E6*(I6))</f>
@@ -671,14 +671,14 @@
         <v>2</v>
       </c>
       <c r="G7" t="n">
-        <v>399.514</v>
+        <v>369.885</v>
       </c>
       <c r="H7" s="11">
         <f>SUM(E7*(I7))</f>
         <v/>
       </c>
       <c r="I7" s="10" t="n">
-        <v>0.1002</v>
+        <v>0.1254</v>
       </c>
     </row>
     <row customHeight="1" ht="23.4" r="16" s="15" spans="1:12">

</xml_diff>